<commit_message>
Tested the code with a subset of real data and compared the output with expected one. Everything checks out and now the code is good to be used for production
</commit_message>
<xml_diff>
--- a/random_stuff/percentile/example_input.xlsx
+++ b/random_stuff/percentile/example_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phyo.thiha\Desktop\others\random_stuff\percentile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1DF6CE-EDAD-4668-B824-082D81E2EF5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="28755" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="28755" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
   <si>
     <t>Year</t>
   </si>
@@ -64,13 +70,31 @@
   </si>
   <si>
     <t>C10</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +131,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +217,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +269,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,16 +462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,10 +482,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -427,11 +498,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -441,11 +515,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -455,11 +532,14 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -469,11 +549,14 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -483,11 +566,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -497,11 +583,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -511,11 +600,14 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -525,11 +617,14 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -539,11 +634,14 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -553,11 +651,14 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -567,11 +668,14 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -581,11 +685,14 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2019</v>
       </c>
@@ -595,11 +702,14 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -609,11 +719,14 @@
       <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -623,11 +736,14 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -637,11 +753,14 @@
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -651,11 +770,14 @@
       <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -665,11 +787,14 @@
       <c r="C19" t="s">
         <v>13</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -679,11 +804,14 @@
       <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -693,7 +821,10 @@
       <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
         <v>6</v>
       </c>
     </row>
@@ -703,24 +834,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>